<commit_message>
added final sheets and data
</commit_message>
<xml_diff>
--- a/Data/virus_comparison.xlsx
+++ b/Data/virus_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Ly\Documents\Programming\COVID19\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47202304-8ACD-4D1C-A079-CE94F5176B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C07F674-F350-43AF-AB33-839DAE5E7425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="1590" windowWidth="26430" windowHeight="18480" xr2:uid="{F673E4EA-9B45-433D-BE89-7D7FA9743D01}"/>
+    <workbookView xWindow="17895" yWindow="1650" windowWidth="29235" windowHeight="18900" xr2:uid="{F673E4EA-9B45-433D-BE89-7D7FA9743D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92214AE7-A748-4497-BD83-6ADD1148DB4D}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,19 +672,19 @@
         <v>2020</v>
       </c>
       <c r="C6" s="8">
-        <v>53930000</v>
+        <v>75670000</v>
       </c>
       <c r="D6" s="1">
-        <v>1310000</v>
+        <v>1670000</v>
       </c>
       <c r="E6" s="2">
-        <v>3.5999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F6" s="1">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G6" s="5">
-        <v>44150</v>
+        <v>44185</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>21</v>

</xml_diff>